<commit_message>
feat: add scheduler example and alarm script
</commit_message>
<xml_diff>
--- a/Config/Localisation.xlsx
+++ b/Config/Localisation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\DemoVersion\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shk_e\Documents\Sources\Siview Community Template Application\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="370">
   <si>
     <t>Original</t>
   </si>
@@ -1111,6 +1111,24 @@
   </si>
   <si>
     <t>ELEMENTS IN MAINTENANCE STATE</t>
+  </si>
+  <si>
+    <t>PILOTAGE VENTILATION</t>
+  </si>
+  <si>
+    <t>PLANNING DE VENTILATION</t>
+  </si>
+  <si>
+    <t>VENTILATION CONTROL</t>
+  </si>
+  <si>
+    <t>VENTILATION SCHEDULE</t>
+  </si>
+  <si>
+    <t>GESTIONNAIRE DE PLANNING</t>
+  </si>
+  <si>
+    <t>SCHEDULE MANAGER</t>
   </si>
 </sst>
 </file>
@@ -1437,10 +1455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B184"/>
+  <dimension ref="A1:B187"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A150" workbookViewId="0">
-      <selection activeCell="B185" sqref="B185"/>
+      <selection activeCell="B188" sqref="B188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -2921,6 +2939,30 @@
         <v>363</v>
       </c>
     </row>
+    <row r="185" spans="1:2">
+      <c r="A185" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="B185" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2">
+      <c r="A186" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="B186" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2">
+      <c r="A187" t="s">
+        <v>368</v>
+      </c>
+      <c r="B187" t="s">
+        <v>369</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
feat: add push button action and client/server status examples
</commit_message>
<xml_diff>
--- a/Config/Localisation.xlsx
+++ b/Config/Localisation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="18690"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4870"/>
   </bookViews>
   <sheets>
     <sheet name="Translations" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="393">
   <si>
     <t>Original</t>
   </si>
@@ -213,6 +213,12 @@
     <t xml:space="preserve">  ACTIVE ALARMS</t>
   </si>
   <si>
+    <t xml:space="preserve">  FONCTIONS AVANCÉES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ADVANCED FUNCTIONS</t>
+  </si>
+  <si>
     <t>LANCEMENT SCRIPT INFOS PC</t>
   </si>
   <si>
@@ -222,6 +228,9 @@
     <t>Exemple d'utilisation d'un script pour la récupération d'infos systèmes.</t>
   </si>
   <si>
+    <t>Example of using a script for retrieving system informations.</t>
+  </si>
+  <si>
     <t>Mémoire Virtuelle</t>
   </si>
   <si>
@@ -267,6 +276,9 @@
     <t>Exemple de passage de paramètres à une même popup + Verrou boutons.</t>
   </si>
   <si>
+    <t>Example of sending parameters to the same popup + Buttons Lock.</t>
+  </si>
+  <si>
     <t>POPUP MEMOIRE VIRTUELLE</t>
   </si>
   <si>
@@ -906,183 +918,171 @@
     <t>Dans le 2eme exemple, la valeur de substitution provient d'une variable.</t>
   </si>
   <si>
+    <t>In the second example, the substituted value is provided by a variable.</t>
+  </si>
+  <si>
     <t>CHANGEMENT DE LANGUE</t>
   </si>
   <si>
+    <t>LANGUAGE CHANGE</t>
+  </si>
+  <si>
     <t>CONFIGURATION LOGICIELLE</t>
   </si>
   <si>
+    <t>SOFTWARE CONFIGURATION</t>
+  </si>
+  <si>
     <t>EDITEUR DE CONFIGURATION</t>
   </si>
   <si>
+    <t>CONFIGURATION EDITOR</t>
+  </si>
+  <si>
     <t>EDITEUR DE SYNOPTIQUE</t>
   </si>
   <si>
+    <t>SYNOPTIC EDITOR</t>
+  </si>
+  <si>
     <t>GESTION DE L'AUTHENTIFICATION</t>
   </si>
   <si>
+    <t>AUTHENTICATION MANAGER</t>
+  </si>
+  <si>
     <t>EDITEUR DES TACHES</t>
   </si>
   <si>
+    <t>TASKS EDITOR</t>
+  </si>
+  <si>
     <t>DECONNEXION UTILISATEUR</t>
   </si>
   <si>
+    <t>USER LOGOFF</t>
+  </si>
+  <si>
     <t>PROGRAMME EXTERNE</t>
   </si>
   <si>
+    <t>EXTERNAL PROGRAM</t>
+  </si>
+  <si>
     <t>IMPRESSION ECRAN</t>
   </si>
   <si>
+    <t>PRINT SCREEN</t>
+  </si>
+  <si>
     <t>QUITTER SIVIEW</t>
   </si>
   <si>
+    <t>EXIT SIVIEW</t>
+  </si>
+  <si>
     <t>ECRITURES DE VARIABLES</t>
   </si>
   <si>
+    <t>WRITING VARIABLES</t>
+  </si>
+  <si>
     <t>INVERSION DE L'ETAT</t>
   </si>
   <si>
+    <t>INVERT STATE</t>
+  </si>
+  <si>
     <t>SAISIE MANUELLE</t>
   </si>
   <si>
+    <t>USER INPUT</t>
+  </si>
+  <si>
     <t>IMPULSION</t>
   </si>
   <si>
+    <t>PULSE</t>
+  </si>
+  <si>
     <t>LISTE DE SELECTION</t>
   </si>
   <si>
+    <t>SELECTION LIST</t>
+  </si>
+  <si>
     <t>TABLEAUX</t>
   </si>
   <si>
+    <t>TABLES</t>
+  </si>
+  <si>
     <t>ETAT DES VANNES</t>
   </si>
   <si>
+    <t>VALVES STATE</t>
+  </si>
+  <si>
     <t>VANNES EN DEFAUTS</t>
   </si>
   <si>
+    <t>VALVES FAILURE</t>
+  </si>
+  <si>
     <t>REGLAGE CONSIGNES PROCESS</t>
   </si>
   <si>
+    <t>PROCESS INPUTS SETTING</t>
+  </si>
+  <si>
     <t>APPEL D'UN SCRIPT UTILISATEUR</t>
   </si>
   <si>
+    <t>USER SCRIPT UTILISATION</t>
+  </si>
+  <si>
     <t>OUVERTURE DE POPUP</t>
   </si>
   <si>
+    <t>POPUP ACTION</t>
+  </si>
+  <si>
     <t>SUBSTITUTION DE PARAMETRES</t>
   </si>
   <si>
+    <t>SUBSTITUTE PARAMETERS</t>
+  </si>
+  <si>
     <t>L'accès à ces commandes est protégé.</t>
   </si>
   <si>
+    <t>Access to these commands is protected.</t>
+  </si>
+  <si>
     <t>Le mot de passe «Admin» est «kscada».</t>
   </si>
   <si>
+    <t>The «Admin» password is «kscada».</t>
+  </si>
+  <si>
     <t>Regarder le paramètre «Niveau d'accès» dans l'onglet «Actions» des boutons.</t>
   </si>
   <si>
+    <t>Look at the parameter «Niveau d'accès» in the buttons «Actions» tab.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Toutes ces commandes systèmes sont ignorées par le client web. </t>
   </si>
   <si>
+    <t>All these system commands are ignored by the webclient.</t>
+  </si>
+  <si>
     <t>Remarques :</t>
   </si>
   <si>
-    <t xml:space="preserve">  ADVANCED FUNCTIONS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  FONCTIONS AVANCÉES</t>
-  </si>
-  <si>
-    <t>Example of using a script for retrieving system informations.</t>
-  </si>
-  <si>
-    <t>Example of sending parameters to the same popup + Buttons Lock.</t>
-  </si>
-  <si>
-    <t>In the second example, the substituted value is provided by a variable.</t>
-  </si>
-  <si>
-    <t>LANGUAGE CHANGE</t>
-  </si>
-  <si>
-    <t>SOFTWARE CONFIGURATION</t>
-  </si>
-  <si>
-    <t>CONFIGURATION EDITOR</t>
-  </si>
-  <si>
-    <t>SYNOPTIC EDITOR</t>
-  </si>
-  <si>
-    <t>AUTHENTICATION MANAGER</t>
-  </si>
-  <si>
-    <t>TASKS EDITOR</t>
-  </si>
-  <si>
-    <t>USER LOGOFF</t>
-  </si>
-  <si>
-    <t>EXTERNAL PROGRAM</t>
-  </si>
-  <si>
-    <t>PRINT SCREEN</t>
-  </si>
-  <si>
-    <t>EXIT SIVIEW</t>
-  </si>
-  <si>
-    <t>WRITING VARIABLES</t>
-  </si>
-  <si>
-    <t>INVERT STATE</t>
-  </si>
-  <si>
-    <t>USER INPUT</t>
-  </si>
-  <si>
-    <t>PULSE</t>
-  </si>
-  <si>
-    <t>SELECTION LIST</t>
-  </si>
-  <si>
-    <t>TABLES</t>
-  </si>
-  <si>
-    <t>VALVES STATE</t>
-  </si>
-  <si>
-    <t>VALVES FAILURE</t>
-  </si>
-  <si>
-    <t>PROCESS INPUTS SETTING</t>
-  </si>
-  <si>
-    <t>USER SCRIPT UTILISATION</t>
-  </si>
-  <si>
-    <t>POPUP ACTION</t>
-  </si>
-  <si>
-    <t>SUBSTITUTE PARAMETERS</t>
-  </si>
-  <si>
-    <t>Access to these commands is protected.</t>
-  </si>
-  <si>
-    <t>The «Admin» password is «kscada».</t>
-  </si>
-  <si>
-    <t>Look at the parameter «Niveau d'accès» in the buttons «Actions» tab.</t>
-  </si>
-  <si>
     <t>Remarks :</t>
   </si>
   <si>
-    <t>All these system commands are ignored by the webclient.</t>
-  </si>
-  <si>
     <t>Saisissez une valeur</t>
   </si>
   <si>
@@ -1092,12 +1092,12 @@
     <t>VALEUR DIX</t>
   </si>
   <si>
+    <t>VALUE OF TEN</t>
+  </si>
+  <si>
     <t>VALEUR TRENTE</t>
   </si>
   <si>
-    <t>VALUE OF TEN</t>
-  </si>
-  <si>
     <t>VALUE OF THIRTY</t>
   </si>
   <si>
@@ -1116,12 +1116,12 @@
     <t>PILOTAGE VENTILATION</t>
   </si>
   <si>
+    <t>VENTILATION CONTROL</t>
+  </si>
+  <si>
     <t>PLANNING DE VENTILATION</t>
   </si>
   <si>
-    <t>VENTILATION CONTROL</t>
-  </si>
-  <si>
     <t>VENTILATION SCHEDULE</t>
   </si>
   <si>
@@ -1129,13 +1129,82 @@
   </si>
   <si>
     <t>SCHEDULE MANAGER</t>
+  </si>
+  <si>
+    <t>INHIBITION DES ALARMES</t>
+  </si>
+  <si>
+    <t>POUSSOIR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  MISE EN RÉSEAU</t>
+  </si>
+  <si>
+    <t>MODE CLIENT/SERVEUR</t>
+  </si>
+  <si>
+    <t>AUTONOME</t>
+  </si>
+  <si>
+    <t>SERVEUR PRIMAIRE</t>
+  </si>
+  <si>
+    <t>SERVEUR SECONDAIRE</t>
+  </si>
+  <si>
+    <t>STATUTS</t>
+  </si>
+  <si>
+    <t>PRIMAIRE CONNECTÉ</t>
+  </si>
+  <si>
+    <t>SECONDAIRE CONNECTÉ</t>
+  </si>
+  <si>
+    <t>CONNEXION EQUIPEMENT</t>
+  </si>
+  <si>
+    <t>ACTIVER LE MODE RESEAU POUR AFFICHER LES STATUTS</t>
+  </si>
+  <si>
+    <t>ALARMS INHIBITION</t>
+  </si>
+  <si>
+    <t>PUSH BUTTON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  NETWORK</t>
+  </si>
+  <si>
+    <t>CLIENT/SERVER MODE</t>
+  </si>
+  <si>
+    <t>STANDALONE</t>
+  </si>
+  <si>
+    <t>PRIMARY SERVER</t>
+  </si>
+  <si>
+    <t>SECONDARY SERVER</t>
+  </si>
+  <si>
+    <t>PRIMARY CONNECTED</t>
+  </si>
+  <si>
+    <t>SECONDARY CONNECTED</t>
+  </si>
+  <si>
+    <t>DEVICE CONNECTED</t>
+  </si>
+  <si>
+    <t>ENABLE NETWORK MODE TO DISPLAY THE STATUS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -1144,11 +1213,6 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1171,10 +1235,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1455,10 +1518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B187"/>
+  <dimension ref="A1:B199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A150" workbookViewId="0">
-      <selection activeCell="B188" sqref="B188"/>
+    <sheetView tabSelected="1" topLeftCell="A187" workbookViewId="0">
+      <selection activeCell="B198" sqref="B198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -1725,1185 +1788,1185 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>323</v>
+        <v>64</v>
       </c>
       <c r="B33" t="s">
-        <v>322</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B34" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B35" t="s">
-        <v>324</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B36" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B37" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B38" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B39" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B40" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B41" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B42" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B43" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B44" t="s">
-        <v>325</v>
+        <v>85</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B45" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B46" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B47" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B48" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B49" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B50" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B51" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="B52" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B53" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="B54" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="B55" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="B56" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B57" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B58" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B59" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B60" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B61" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B62" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B63" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B64" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="B65" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B66" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B67" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B68" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B69" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="B70" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B71" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="B72" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="B73" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="B74" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B75" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B76" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B77" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="B78" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="B79" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="B80" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="B81" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="B82" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="B83" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="B84" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="B85" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="B86" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="B87" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="B88" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="B89" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="B90" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="B91" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="B92" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="B93" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="B94" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="B95" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="B96" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="B97" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="B98" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="B99" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="B100" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="B101" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="102" spans="1:2">
       <c r="A102" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="B102" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="B103" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="B104" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="B105" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="B106" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="B107" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="B108" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="B109" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B110" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="B111" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="B112" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="B113" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="B114" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="B115" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="B116" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="B117" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="B118" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="B119" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="B120" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="B121" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="B122" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="B123" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="B124" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="B125" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="B126" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="B127" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="B128" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
     </row>
     <row r="129" spans="1:2">
       <c r="A129" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="B129" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="B130" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
     </row>
     <row r="131" spans="1:2">
       <c r="A131" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="B131" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="A132" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="B132" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="B133" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="B134" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="B135" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="B136" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="B137" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="B138" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="B139" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="B140" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="B141" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="B142" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="B143" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="B144" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="B145" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="B146" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
     </row>
     <row r="147" spans="1:2">
       <c r="A147" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="B147" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="B148" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="B149" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="B150" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
     </row>
     <row r="151" spans="1:2">
       <c r="A151" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="B151" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="B152" t="s">
-        <v>326</v>
+        <v>299</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="B153" t="s">
-        <v>327</v>
+        <v>301</v>
       </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154" t="s">
-        <v>296</v>
+        <v>302</v>
       </c>
       <c r="B154" t="s">
-        <v>328</v>
+        <v>303</v>
       </c>
     </row>
     <row r="155" spans="1:2">
       <c r="A155" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="B155" t="s">
-        <v>329</v>
+        <v>305</v>
       </c>
     </row>
     <row r="156" spans="1:2">
       <c r="A156" t="s">
-        <v>298</v>
+        <v>306</v>
       </c>
       <c r="B156" t="s">
-        <v>330</v>
+        <v>307</v>
       </c>
     </row>
     <row r="157" spans="1:2">
       <c r="A157" t="s">
-        <v>299</v>
+        <v>308</v>
       </c>
       <c r="B157" t="s">
-        <v>331</v>
+        <v>309</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158" t="s">
-        <v>300</v>
+        <v>310</v>
       </c>
       <c r="B158" t="s">
-        <v>332</v>
+        <v>311</v>
       </c>
     </row>
     <row r="159" spans="1:2">
       <c r="A159" t="s">
-        <v>301</v>
+        <v>312</v>
       </c>
       <c r="B159" t="s">
-        <v>333</v>
+        <v>313</v>
       </c>
     </row>
     <row r="160" spans="1:2">
       <c r="A160" t="s">
-        <v>302</v>
+        <v>314</v>
       </c>
       <c r="B160" t="s">
-        <v>334</v>
+        <v>315</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" t="s">
-        <v>303</v>
+        <v>316</v>
       </c>
       <c r="B161" t="s">
-        <v>335</v>
+        <v>317</v>
       </c>
     </row>
     <row r="162" spans="1:2">
       <c r="A162" t="s">
-        <v>304</v>
+        <v>318</v>
       </c>
       <c r="B162" t="s">
-        <v>336</v>
+        <v>319</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" t="s">
-        <v>305</v>
+        <v>320</v>
       </c>
       <c r="B163" t="s">
-        <v>337</v>
+        <v>321</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" t="s">
-        <v>306</v>
+        <v>322</v>
       </c>
       <c r="B164" t="s">
-        <v>338</v>
+        <v>323</v>
       </c>
     </row>
     <row r="165" spans="1:2">
       <c r="A165" t="s">
-        <v>307</v>
+        <v>324</v>
       </c>
       <c r="B165" t="s">
-        <v>339</v>
+        <v>325</v>
       </c>
     </row>
     <row r="166" spans="1:2">
       <c r="A166" t="s">
-        <v>308</v>
+        <v>326</v>
       </c>
       <c r="B166" t="s">
-        <v>340</v>
+        <v>327</v>
       </c>
     </row>
     <row r="167" spans="1:2">
       <c r="A167" t="s">
-        <v>309</v>
+        <v>328</v>
       </c>
       <c r="B167" t="s">
-        <v>341</v>
+        <v>329</v>
       </c>
     </row>
     <row r="168" spans="1:2">
       <c r="A168" t="s">
-        <v>310</v>
+        <v>330</v>
       </c>
       <c r="B168" t="s">
-        <v>342</v>
+        <v>331</v>
       </c>
     </row>
     <row r="169" spans="1:2">
       <c r="A169" t="s">
-        <v>311</v>
+        <v>332</v>
       </c>
       <c r="B169" t="s">
-        <v>343</v>
+        <v>333</v>
       </c>
     </row>
     <row r="170" spans="1:2">
       <c r="A170" t="s">
-        <v>312</v>
+        <v>334</v>
       </c>
       <c r="B170" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
     </row>
     <row r="171" spans="1:2">
       <c r="A171" t="s">
-        <v>313</v>
+        <v>336</v>
       </c>
       <c r="B171" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
     </row>
     <row r="172" spans="1:2">
       <c r="A172" t="s">
-        <v>314</v>
+        <v>338</v>
       </c>
       <c r="B172" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
     </row>
     <row r="173" spans="1:2">
       <c r="A173" t="s">
-        <v>315</v>
+        <v>340</v>
       </c>
       <c r="B173" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
     </row>
     <row r="174" spans="1:2">
       <c r="A174" t="s">
-        <v>316</v>
+        <v>342</v>
       </c>
       <c r="B174" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
     </row>
     <row r="175" spans="1:2">
       <c r="A175" t="s">
-        <v>317</v>
-      </c>
-      <c r="B175" s="2" t="s">
-        <v>349</v>
+        <v>344</v>
+      </c>
+      <c r="B175" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="176" spans="1:2">
-      <c r="A176" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="B176" s="2" t="s">
-        <v>350</v>
+      <c r="A176" t="s">
+        <v>346</v>
+      </c>
+      <c r="B176" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="177" spans="1:2">
       <c r="A177" t="s">
-        <v>319</v>
-      </c>
-      <c r="B177" s="2" t="s">
-        <v>351</v>
+        <v>348</v>
+      </c>
+      <c r="B177" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="178" spans="1:2">
       <c r="A178" t="s">
-        <v>320</v>
-      </c>
-      <c r="B178" s="2" t="s">
-        <v>353</v>
+        <v>350</v>
+      </c>
+      <c r="B178" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="179" spans="1:2">
       <c r="A179" t="s">
-        <v>321</v>
-      </c>
-      <c r="B179" s="2" t="s">
         <v>352</v>
+      </c>
+      <c r="B179" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="180" spans="1:2">
       <c r="A180" t="s">
         <v>354</v>
       </c>
-      <c r="B180" s="2" t="s">
+      <c r="B180" t="s">
         <v>355</v>
       </c>
     </row>
@@ -2911,45 +2974,45 @@
       <c r="A181" t="s">
         <v>356</v>
       </c>
-      <c r="B181" s="2" t="s">
-        <v>358</v>
+      <c r="B181" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="182" spans="1:2">
       <c r="A182" t="s">
-        <v>357</v>
-      </c>
-      <c r="B182" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B182" t="s">
         <v>359</v>
       </c>
     </row>
     <row r="183" spans="1:2">
-      <c r="A183" s="2" t="s">
+      <c r="A183" t="s">
         <v>360</v>
       </c>
-      <c r="B183" s="2" t="s">
+      <c r="B183" t="s">
         <v>361</v>
       </c>
     </row>
     <row r="184" spans="1:2">
-      <c r="A184" s="2" t="s">
+      <c r="A184" t="s">
         <v>362</v>
       </c>
-      <c r="B184" s="2" t="s">
+      <c r="B184" t="s">
         <v>363</v>
       </c>
     </row>
     <row r="185" spans="1:2">
-      <c r="A185" s="2" t="s">
+      <c r="A185" t="s">
         <v>364</v>
       </c>
       <c r="B185" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2">
+      <c r="A186" t="s">
         <v>366</v>
-      </c>
-    </row>
-    <row r="186" spans="1:2">
-      <c r="A186" s="2" t="s">
-        <v>365</v>
       </c>
       <c r="B186" t="s">
         <v>367</v>
@@ -2963,8 +3026,103 @@
         <v>369</v>
       </c>
     </row>
+    <row r="188" spans="1:2">
+      <c r="A188" t="s">
+        <v>370</v>
+      </c>
+      <c r="B188" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2">
+      <c r="A189" t="s">
+        <v>371</v>
+      </c>
+      <c r="B189" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2">
+      <c r="A190" t="s">
+        <v>372</v>
+      </c>
+      <c r="B190" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2">
+      <c r="A191" t="s">
+        <v>373</v>
+      </c>
+      <c r="B191" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2">
+      <c r="A192" t="s">
+        <v>374</v>
+      </c>
+      <c r="B192" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2">
+      <c r="A193" t="s">
+        <v>375</v>
+      </c>
+      <c r="B193" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2">
+      <c r="A194" t="s">
+        <v>376</v>
+      </c>
+      <c r="B194" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2">
+      <c r="A195" t="s">
+        <v>377</v>
+      </c>
+      <c r="B195" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2">
+      <c r="A196" t="s">
+        <v>378</v>
+      </c>
+      <c r="B196" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2">
+      <c r="A197" t="s">
+        <v>379</v>
+      </c>
+      <c r="B197" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2">
+      <c r="A198" t="s">
+        <v>380</v>
+      </c>
+      <c r="B198" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2">
+      <c r="A199" t="s">
+        <v>381</v>
+      </c>
+      <c r="B199" t="s">
+        <v>392</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: add logviewer in alarm page
</commit_message>
<xml_diff>
--- a/Config/Localisation.xlsx
+++ b/Config/Localisation.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="427">
   <si>
     <t>Original</t>
   </si>
@@ -201,18 +201,6 @@
     <t>Settings</t>
   </si>
   <si>
-    <t xml:space="preserve">  HISTORIQUE DES ALARMES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  ALARMS HISTORY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  ALARMES ACTIVES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  ACTIVE ALARMS</t>
-  </si>
-  <si>
     <t xml:space="preserve">  FONCTIONS AVANCÉES</t>
   </si>
   <si>
@@ -1288,6 +1276,30 @@
   </si>
   <si>
     <t>PRODUCTION REPORT</t>
+  </si>
+  <si>
+    <t>JOURNAL D'EVENEMENTS</t>
+  </si>
+  <si>
+    <t>EVENT LOG</t>
+  </si>
+  <si>
+    <t>HISTORIQUE DES ALARMES</t>
+  </si>
+  <si>
+    <t>ALARMES ACTIVES</t>
+  </si>
+  <si>
+    <t>ALARMS HISTORY</t>
+  </si>
+  <si>
+    <t>ACTIVE ALARMS</t>
+  </si>
+  <si>
+    <t>HISTORIQUES</t>
+  </si>
+  <si>
+    <t>HISTORY</t>
   </si>
 </sst>
 </file>
@@ -1608,10 +1620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B214"/>
+  <dimension ref="A1:B216"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
-      <selection activeCell="A217" sqref="A217"/>
+    <sheetView tabSelected="1" topLeftCell="A196" workbookViewId="0">
+      <selection activeCell="B217" sqref="B217"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -1862,1474 +1874,1490 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>60</v>
+        <v>421</v>
       </c>
       <c r="B31" t="s">
-        <v>61</v>
+        <v>423</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>62</v>
+        <v>422</v>
       </c>
       <c r="B32" t="s">
-        <v>63</v>
+        <v>424</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B33" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B34" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B35" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B36" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B37" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B38" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B39" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B40" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B41" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B42" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B43" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B44" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B45" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B46" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B47" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B48" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B49" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B50" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B51" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B52" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B53" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B54" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B55" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B56" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B57" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B58" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B59" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B60" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B61" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B62" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B63" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B64" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B65" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B66" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B67" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B68" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B69" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B70" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B71" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B72" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B73" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B74" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B75" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B76" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B77" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B78" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B79" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B80" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B81" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B82" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B83" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B84" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B85" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B86" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B87" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B88" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B89" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B90" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B91" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B92" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B93" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B94" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B95" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B96" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B97" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B98" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B99" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B100" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B101" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="102" spans="1:2">
       <c r="A102" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B102" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B103" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B104" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B105" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B106" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B107" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B108" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B109" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B110" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B111" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B112" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B113" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B114" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B115" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B116" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B117" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B118" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B119" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B120" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B121" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B122" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B123" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B124" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B125" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B126" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B127" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B128" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="129" spans="1:2">
       <c r="A129" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B129" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B130" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="131" spans="1:2">
       <c r="A131" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B131" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="A132" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B132" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="B133" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B134" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="B135" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B136" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="B137" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B138" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="B139" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B140" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B141" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B142" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="B143" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="B144" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="B145" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B146" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="147" spans="1:2">
       <c r="A147" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="B147" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="B148" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B149" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B150" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="151" spans="1:2">
       <c r="A151" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B151" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B152" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B153" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B154" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="155" spans="1:2">
       <c r="A155" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B155" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="156" spans="1:2">
       <c r="A156" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="B156" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="157" spans="1:2">
       <c r="A157" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B157" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="B158" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="159" spans="1:2">
       <c r="A159" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B159" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="160" spans="1:2">
       <c r="A160" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="B160" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B161" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="162" spans="1:2">
       <c r="A162" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="B162" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B163" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="B164" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="165" spans="1:2">
       <c r="A165" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="B165" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="166" spans="1:2">
       <c r="A166" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="B166" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="167" spans="1:2">
       <c r="A167" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="B167" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="168" spans="1:2">
       <c r="A168" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="B168" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="169" spans="1:2">
       <c r="A169" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="B169" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="170" spans="1:2">
       <c r="A170" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="B170" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="171" spans="1:2">
       <c r="A171" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B171" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="172" spans="1:2">
       <c r="A172" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="B172" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="173" spans="1:2">
       <c r="A173" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B173" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="174" spans="1:2">
       <c r="A174" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="B174" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
     </row>
     <row r="175" spans="1:2">
       <c r="A175" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="B175" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="176" spans="1:2">
       <c r="A176" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="B176" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="177" spans="1:2">
       <c r="A177" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="B177" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="178" spans="1:2">
       <c r="A178" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="B178" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
     </row>
     <row r="179" spans="1:2">
       <c r="A179" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="B179" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
     </row>
     <row r="180" spans="1:2">
       <c r="A180" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="B180" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="181" spans="1:2">
       <c r="A181" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="B181" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="182" spans="1:2">
       <c r="A182" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="B182" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="183" spans="1:2">
       <c r="A183" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="B183" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
     </row>
     <row r="184" spans="1:2">
       <c r="A184" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="B184" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="185" spans="1:2">
       <c r="A185" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="B185" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="186" spans="1:2">
       <c r="A186" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="B186" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="187" spans="1:2">
       <c r="A187" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="B187" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="188" spans="1:2">
       <c r="A188" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="B188" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
     </row>
     <row r="189" spans="1:2">
       <c r="A189" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="B189" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
     </row>
     <row r="190" spans="1:2">
       <c r="A190" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="B190" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
     </row>
     <row r="191" spans="1:2">
       <c r="A191" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="B191" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
     </row>
     <row r="192" spans="1:2">
       <c r="A192" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="B192" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
     </row>
     <row r="193" spans="1:2">
       <c r="A193" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="B193" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="194" spans="1:2">
       <c r="A194" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="B194" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="195" spans="1:2">
       <c r="A195" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="B195" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="196" spans="1:2">
       <c r="A196" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="B196" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="197" spans="1:2">
       <c r="A197" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="B197" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="198" spans="1:2">
       <c r="A198" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="B198" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
     </row>
     <row r="199" spans="1:2">
       <c r="A199" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="B199" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="200" spans="1:2">
       <c r="A200" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="B200" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="201" spans="1:2">
       <c r="A201" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="B201" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
     </row>
     <row r="202" spans="1:2">
       <c r="A202" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="B202" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="203" spans="1:2">
       <c r="A203" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="B203" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
     <row r="204" spans="1:2">
       <c r="A204" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="B204" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="205" spans="1:2">
       <c r="A205" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="B205" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="206" spans="1:2">
       <c r="A206" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="B206" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
     </row>
     <row r="207" spans="1:2">
       <c r="A207" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="B207" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
     </row>
     <row r="208" spans="1:2">
       <c r="A208" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="B208" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
     </row>
     <row r="209" spans="1:2">
       <c r="A209" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="B209" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
     </row>
     <row r="210" spans="1:2">
       <c r="A210" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="B210" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
     <row r="211" spans="1:2">
       <c r="A211" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="B211" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
     </row>
     <row r="212" spans="1:2">
       <c r="A212" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="B212" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
     </row>
     <row r="213" spans="1:2">
       <c r="A213" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="B213" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
     </row>
     <row r="214" spans="1:2">
       <c r="A214" t="s">
+        <v>416</v>
+      </c>
+      <c r="B214" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2">
+      <c r="A215" t="s">
+        <v>419</v>
+      </c>
+      <c r="B215" t="s">
         <v>420</v>
       </c>
-      <c r="B214" t="s">
-        <v>422</v>
+    </row>
+    <row r="216" spans="1:2">
+      <c r="A216" t="s">
+        <v>425</v>
+      </c>
+      <c r="B216" t="s">
+        <v>426</v>
       </c>
     </row>
   </sheetData>

</xml_diff>